<commit_message>
MEDI2101 updates to week 9 and 10 material
</commit_message>
<xml_diff>
--- a/images/ABS2017_3303.xlsx
+++ b/images/ABS2017_3303.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://mqoutlook-my.sharepoint.com/personal/mark_butlin_mq_edu_au/Documents/presentations/images/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="4" documentId="13_ncr:1_{DF9BFAEB-5F27-419F-9626-7EB45EC6C20D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{171A8B37-C1A3-4310-95F6-BF3EFF29EBBC}"/>
+  <xr:revisionPtr revIDLastSave="6" documentId="13_ncr:1_{DF9BFAEB-5F27-419F-9626-7EB45EC6C20D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{54D9FDE1-4D03-4B67-B4D0-570AD6A6A4CA}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-18120" windowWidth="29040" windowHeight="18240" xr2:uid="{DBE8A0A3-016C-4DD5-9F7B-219B06E3A97A}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{DBE8A0A3-016C-4DD5-9F7B-219B06E3A97A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -771,9 +771,7 @@
     <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
-    <a:solidFill>
-      <a:schemeClr val="bg1"/>
-    </a:solidFill>
+    <a:noFill/>
     <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
       <a:noFill/>
       <a:round/>

</xml_diff>